<commit_message>
deptment code label changes in employee import excel
</commit_message>
<xml_diff>
--- a/ezyformsfrontend/public/Employee_import.xlsx
+++ b/ezyformsfrontend/public/Employee_import.xlsx
@@ -10,17 +10,17 @@
   <sheets>
     <sheet name="Ezy Employee" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Company Field</t>
   </si>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Emp Phone</t>
   </si>
   <si>
-    <t xml:space="preserve">Department</t>
+    <t xml:space="preserve">Department Code</t>
   </si>
   <si>
     <t xml:space="preserve">Designation</t>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">Reporting Designation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRR</t>
   </si>
 </sst>
 </file>
@@ -56,9 +59,9 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
-    <font>
-      <sz val="11"/>
+  <fonts count="4">
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -78,19 +81,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -135,16 +125,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -165,41 +151,57 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10 G5 F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.3671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.89"/>
+  </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>